<commit_message>
Modified DSL for PB tests
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBPB_Battery.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBPB_Battery.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$1:$K$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$1:$K$13</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -57,49 +57,7 @@
     <t>Connect Device with WIFI</t>
   </si>
   <si>
-    <t>Battery
-  Indicator-JS-4.0</t>
-  </si>
-  <si>
     <t>Change Start page</t>
-  </si>
-  <si>
-    <t>Battery visible with Battery Event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(PB_battery_test_link);
-validate2;
-SelectTestToRun(VT056_1172_string);
-ClickRunTest(runtest_top_xpath);
-wait(3);
-TakeScreenshot(VT056_1172);
-validate3;
-wait(3);
-validate4;
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Pocket Browser Tests
-};
-validate2
-{
-validate_PageTitle=PB Battery Test
-};
-validate3
-{
-validate_Screenshot=VT056_1172
-};
-validate4
-{
-validate_Result=AC: 1
-validate_Result=main:
-validate_Result=backup:
-validate_Result=Count:
-};</t>
   </si>
   <si>
     <t xml:space="preserve">Battery visible </t>
@@ -615,41 +573,6 @@
     <t>Battery Event</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(PB_battery_test_link);
-validate2;
-SelectTestToRun(VT056_1190_string);
-ClickRunTest(runtest_top_xpath);
-wait(3);
-TakeScreenshot(VT056_1190);
-validate3;
-wait(3);
-validate4;
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Pocket Browser Tests
-};
-validate2
-{
-validate_PageTitle=PB Battery Test
-};
-validate3
-{
-validate_Screenshot=VT056_1190
-};
-validate4
-{
-validate_Result=AC: 1
-validate_Result=main:
-validate_Result=backup:
-validate_Result=Count:
-};</t>
-  </si>
-  <si>
     <t>Battery Event with Navigate to URL</t>
   </si>
   <si>
@@ -686,6 +609,37 @@
 ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
 ChangeConfigxml(Configuration/Applications/Application/NPAPI/Preloads,PreloadLegacyActiveX,&lt;PreloadLegacyActiveX value="1"/&gt;);
 PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Pocket Browser Tests
+};
+validate2
+{
+validate_PageTitle=PB Battery Test
+};
+validate4
+{
+validate_Result=AC: 1
+validate_Result=main:
+validate_Result=backup:
+validate_Result=Count:
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(PB_battery_test_link);
+validate2;
+SelectTestToRun(VT056_1190_string);
+ClickRunTest(runtest_top_xpath);
+wait(3);
+validate4;
+</t>
+  </si>
+  <si>
+    <t>PB-Battery</t>
   </si>
 </sst>
 </file>
@@ -1148,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1206,19 +1160,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="2" t="s">
@@ -1227,7 +1181,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="214.5" thickBot="1">
+    <row r="3" spans="1:11" ht="147" thickBot="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1239,16 +1193,16 @@
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1266,13 +1220,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -1299,10 +1253,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1320,16 +1274,16 @@
         <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1347,16 +1301,16 @@
         <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1374,16 +1328,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1401,16 +1355,16 @@
         <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1428,16 +1382,16 @@
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1455,16 +1409,16 @@
         <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1482,16 +1436,16 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1509,16 +1463,16 @@
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1536,16 +1490,16 @@
         <v>10</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1563,16 +1517,16 @@
         <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1590,16 +1544,16 @@
         <v>10</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1617,16 +1571,16 @@
         <v>10</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1644,16 +1598,16 @@
         <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1671,7 +1625,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1686,7 +1640,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="147" thickBot="1">
+    <row r="20" spans="1:11" ht="169.5" thickBot="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1698,22 +1652,22 @@
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="214.5" thickBot="1">
+    <row r="21" spans="1:11" ht="135.75" thickBot="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1725,47 +1679,20 @@
         <v>10</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" ht="135.75" thickBot="1">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>